<commit_message>
Changed Death of HoH form to have the same options for the membership of remaining members as the membership form
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/death_to_hoh.xlsx
+++ b/xforms/xlsforms/death_to_hoh.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="285" windowWidth="21600" windowHeight="9840" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="345" windowWidth="21600" windowHeight="9780" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="151">
   <si>
     <t>type</t>
   </si>
@@ -93,18 +93,12 @@
     <t>relationshipToGroupHead</t>
   </si>
   <si>
-    <t>Mtoto wa Kike/Kiume</t>
-  </si>
-  <si>
     <t>Kaka/Dada</t>
   </si>
   <si>
     <t>Mjukuu</t>
   </si>
   <si>
-    <t>Hakuna Uhusiano</t>
-  </si>
-  <si>
     <t>Uhusiano Mwingine</t>
   </si>
   <si>
@@ -195,9 +189,6 @@
     <t>extId</t>
   </si>
   <si>
-    <t>DEATHTOHOH</t>
-  </si>
-  <si>
     <t>Membership</t>
   </si>
   <si>
@@ -457,6 +448,27 @@
   </si>
   <si>
     <t>no-calendar</t>
+  </si>
+  <si>
+    <t>Mke/Mme</t>
+  </si>
+  <si>
+    <t>Spouse</t>
+  </si>
+  <si>
+    <t>Mtoto Kiume/Kike</t>
+  </si>
+  <si>
+    <t>Mzazi</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>Hakuna Mahusiano</t>
+  </si>
+  <si>
+    <t>death_to_hoh</t>
   </si>
 </sst>
 </file>
@@ -922,7 +934,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -955,9 +967,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1678,11 +1687,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="J14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q5" sqref="Q5"/>
+      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1748,10 +1757,10 @@
         <v>13</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -1819,43 +1828,43 @@
     </row>
     <row r="5" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="K5" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="Q5" s="25"/>
-    </row>
-    <row r="6" spans="1:17" s="23" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="J6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
+      <c r="Q5" s="24"/>
+    </row>
+    <row r="6" spans="1:17" s="22" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="J6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
@@ -1865,7 +1874,7 @@
         <v>20</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H7" s="4" t="b">
         <v>1</v>
@@ -1882,7 +1891,7 @@
         <v>22</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H8" s="4" t="b">
         <v>1</v>
@@ -1896,10 +1905,10 @@
         <v>21</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H9" s="4" t="b">
         <v>1</v>
@@ -1913,10 +1922,10 @@
         <v>21</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H10" s="4" t="b">
         <v>1</v>
@@ -1930,10 +1939,10 @@
         <v>21</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H11" s="4"/>
       <c r="K11" s="4" t="b">
@@ -1945,10 +1954,10 @@
         <v>21</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H12" s="4"/>
       <c r="K12" s="4" t="b">
@@ -1960,10 +1969,10 @@
         <v>21</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H13" s="4" t="b">
         <v>1</v>
@@ -1972,30 +1981,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="H14" s="22"/>
+    <row r="14" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="H14" s="21"/>
     </row>
     <row r="15" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H15" s="5" t="b">
         <v>1</v>
@@ -2003,13 +2012,13 @@
     </row>
     <row r="16" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -2021,16 +2030,16 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -2042,16 +2051,16 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C18" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>77</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -2063,16 +2072,16 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -2084,13 +2093,13 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H20" s="5" t="b">
         <v>1</v>
@@ -2101,13 +2110,13 @@
         <v>21</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H21" s="5" t="b">
         <v>1</v>
@@ -2115,16 +2124,16 @@
     </row>
     <row r="22" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="J22" s="5" t="s">
         <v>119</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>122</v>
       </c>
       <c r="K22" s="5" t="b">
         <v>1</v>
@@ -2132,16 +2141,16 @@
     </row>
     <row r="23" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C23" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H23" s="4" t="b">
         <v>1</v>
@@ -2151,17 +2160,17 @@
       </c>
     </row>
     <row r="24" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="19" t="s">
-        <v>50</v>
+      <c r="A24" s="18" t="s">
+        <v>48</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="P24" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
@@ -2169,10 +2178,10 @@
         <v>21</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -2188,10 +2197,10 @@
         <v>21</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -2210,7 +2219,7 @@
         <v>23</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -2223,13 +2232,13 @@
     </row>
     <row r="28" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -2238,8 +2247,8 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" s="19" t="s">
-        <v>49</v>
+      <c r="A29" s="18" t="s">
+        <v>47</v>
       </c>
       <c r="B29" s="2"/>
       <c r="D29" s="9"/>
@@ -2248,13 +2257,13 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="K30" s="5" t="b">
         <v>1</v>
@@ -2319,10 +2328,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2349,484 +2358,512 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="15">
-        <v>1</v>
-      </c>
-      <c r="C2" s="16" t="s">
+      <c r="B2" s="14">
+        <v>2</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="14">
+        <v>3</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="14">
+        <v>4</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D4" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="14">
+        <v>5</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="14">
+        <v>6</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="14">
+        <v>7</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="14">
+        <v>8</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B9" s="14">
+        <v>9</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="14">
+        <v>1</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="14">
         <v>2</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="15">
+      <c r="C11" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="14">
+        <v>1</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="14">
+        <v>2</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="14">
         <v>3</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="15">
+      <c r="C14" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="14">
         <v>4</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="15">
-        <v>5</v>
-      </c>
-      <c r="C6" s="16" t="s">
+      <c r="C15" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="15">
-        <v>6</v>
-      </c>
-      <c r="C7" s="16" t="s">
+      <c r="C29" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="15">
-        <v>1</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="15">
-        <v>2</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" s="15">
-        <v>1</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" s="15">
-        <v>2</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B12" s="15">
-        <v>3</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B13" s="15">
-        <v>4</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B19" s="15" t="s">
+      <c r="C30" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
     </row>
     <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
     </row>
     <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
     </row>
     <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
     </row>
     <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
     </row>
     <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="13"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
     </row>
     <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
     </row>
     <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="16"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
     </row>
     <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="13"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="13"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2838,8 +2875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2851,30 +2888,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="D1" s="23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" t="s">
         <v>53</v>
       </c>
-      <c r="C1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>140</v>
+      <c r="D2" s="23" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>